<commit_message>
eod 1-30, working on apparent duplication in Agency Completion Search
</commit_message>
<xml_diff>
--- a/Ciudad Completes.xlsx
+++ b/Ciudad Completes.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="150">
   <si>
     <t>ABEL</t>
   </si>
@@ -26,7 +26,7 @@
     <t>agonzalezsa@queretaro.gob.mx</t>
   </si>
   <si>
-    <t>Ciudad</t>
+    <t>Secretaría de Seguridad Ciudadana del Estado de Querétaro</t>
   </si>
   <si>
     <t>ALEJANDRO</t>
@@ -36,6 +36,9 @@
   </si>
   <si>
     <t>alejandrocamposcruz@gmail.com</t>
+  </si>
+  <si>
+    <t>Secretaría de Seguridad Pública de la Ciudad de México</t>
   </si>
   <si>
     <t>ARMANDO</t>
@@ -830,32 +833,32 @@
         <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D4" t="s">
         <v>3</v>
@@ -863,13 +866,13 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D5" t="s">
         <v>3</v>
@@ -877,55 +880,55 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D6" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D7" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D8" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D9" t="s">
         <v>3</v>
@@ -933,13 +936,13 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B10" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C10" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D10" t="s">
         <v>3</v>
@@ -947,41 +950,41 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B11" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C11" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D11" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B12" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C12" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D12" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B13" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C13" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D13" t="s">
         <v>3</v>
@@ -989,13 +992,13 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B14" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C14" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D14" t="s">
         <v>3</v>
@@ -1003,13 +1006,13 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B15" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C15" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D15" t="s">
         <v>3</v>
@@ -1017,41 +1020,41 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B16" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C16" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D16" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B17" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C17" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D17" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B18" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C18" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D18" t="s">
         <v>3</v>
@@ -1059,13 +1062,13 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B19" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C19" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D19" t="s">
         <v>3</v>
@@ -1073,13 +1076,13 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B20" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C20" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D20" t="s">
         <v>3</v>
@@ -1087,13 +1090,13 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B21" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C21" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D21" t="s">
         <v>3</v>
@@ -1101,83 +1104,83 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B22" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C22" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D22" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B23" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C23" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D23" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B24" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C24" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D24" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B25" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C25" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D25" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B26" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C26" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D26" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B27" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C27" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D27" t="s">
         <v>3</v>
@@ -1185,13 +1188,13 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B28" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C28" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D28" t="s">
         <v>3</v>
@@ -1199,27 +1202,27 @@
     </row>
     <row r="29" spans="1:4">
       <c r="A29" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B29" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C29" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D29" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B30" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C30" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D30" t="s">
         <v>3</v>
@@ -1227,13 +1230,13 @@
     </row>
     <row r="31" spans="1:4">
       <c r="A31" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B31" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C31" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D31" t="s">
         <v>3</v>
@@ -1241,41 +1244,41 @@
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B32" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C32" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D32" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B33" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C33" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D33" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B34" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C34" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D34" t="s">
         <v>3</v>
@@ -1286,10 +1289,10 @@
         <v>4</v>
       </c>
       <c r="B35" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C35" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D35" t="s">
         <v>3</v>
@@ -1297,13 +1300,13 @@
     </row>
     <row r="36" spans="1:4">
       <c r="A36" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B36" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C36" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D36" t="s">
         <v>3</v>
@@ -1311,41 +1314,41 @@
     </row>
     <row r="37" spans="1:4">
       <c r="A37" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B37" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C37" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D37" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B38" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C38" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D38" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B39" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C39" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D39" t="s">
         <v>3</v>
@@ -1353,13 +1356,13 @@
     </row>
     <row r="40" spans="1:4">
       <c r="A40" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B40" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C40" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D40" t="s">
         <v>3</v>
@@ -1367,27 +1370,27 @@
     </row>
     <row r="41" spans="1:4">
       <c r="A41" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B41" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C41" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D41" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B42" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C42" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D42" t="s">
         <v>3</v>
@@ -1395,13 +1398,13 @@
     </row>
     <row r="43" spans="1:4">
       <c r="A43" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B43" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C43" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D43" t="s">
         <v>3</v>
@@ -1409,13 +1412,13 @@
     </row>
     <row r="44" spans="1:4">
       <c r="A44" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B44" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C44" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D44" t="s">
         <v>3</v>
@@ -1423,55 +1426,55 @@
     </row>
     <row r="45" spans="1:4">
       <c r="A45" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B45" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C45" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D45" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B46" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C46" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D46" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="47" spans="1:4">
       <c r="A47" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B47" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C47" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D47" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="48" spans="1:4">
       <c r="A48" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B48" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C48" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D48" t="s">
         <v>3</v>
@@ -1479,27 +1482,27 @@
     </row>
     <row r="49" spans="1:4">
       <c r="A49" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B49" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C49" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D49" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="50" spans="1:4">
       <c r="A50" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B50" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C50" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D50" t="s">
         <v>3</v>
@@ -1507,13 +1510,13 @@
     </row>
     <row r="51" spans="1:4">
       <c r="A51" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B51" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C51" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D51" t="s">
         <v>3</v>

</xml_diff>